<commit_message>
Update for 18 Jan
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FE6ED-2F7F-DB4A-A4A1-F9C44C6BB372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27696DBC-E9F3-DB47-95D6-4F6CAE35EA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Reached lesson 5.3</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>Reached lesson 5.4</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>Reached lesson 5.5</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>Completed Lesson 5.8, working on 5.9</t>
   </si>
 </sst>
 </file>
@@ -541,7 +559,7 @@
   <dimension ref="B1:E51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -597,19 +615,37 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>43846</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>43847</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="8">
+        <v>43848</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="6"/>

</xml_diff>

<commit_message>
D17: Completed Fashion MNIST exercise Also adding D16's work
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC12E4D-C452-5347-9912-1F93704FA4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B930843B-1BB1-1A4D-9B8F-A6B42B5692F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Reached lesson 5.11</t>
+  </si>
+  <si>
+    <t>Completed till lesson 5.13</t>
+  </si>
+  <si>
+    <t>D17</t>
   </si>
 </sst>
 </file>
@@ -571,7 +577,7 @@
   <dimension ref="B1:E51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -682,9 +688,15 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="8">
+        <v>43851</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="6"/>

</xml_diff>

<commit_message>
D24: Lesson 6 exercises
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E57B1F-0D8F-8C46-B778-1C9BBD4AB364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C60D6-2C3F-EC43-A435-17EF6BC8F1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,24 @@
   </si>
   <si>
     <t>Completed lesson 5. Started with lesson 6, reached till 6.10</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t>Started working on Intel Image classification problem. Also watched some videos about CNN</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>Out sick</t>
+  </si>
+  <si>
+    <t>D24</t>
+  </si>
+  <si>
+    <t>Completed lessons 6.11 to 6.24</t>
   </si>
 </sst>
 </file>
@@ -597,7 +615,7 @@
   </sheetPr>
   <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B44" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -764,19 +782,37 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="8">
+        <v>43856</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="6"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="8">
+        <v>43857</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="6"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="8">
+        <v>43858</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="6"/>

</xml_diff>

<commit_message>
Completed lesson 6 Convnet exercise
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C60D6-2C3F-EC43-A435-17EF6BC8F1DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70475CC-FF42-C746-9B94-71D46318BC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,30 @@
   </si>
   <si>
     <t>Completed lessons 6.11 to 6.24</t>
+  </si>
+  <si>
+    <t>D25</t>
+  </si>
+  <si>
+    <t>Completed lessons 6.25 to 6.28</t>
+  </si>
+  <si>
+    <t>Completed lessons 6.29 to 6.31</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>Completed lessons 6.32 to 6.34</t>
+  </si>
+  <si>
+    <t>Completed lesson 6(6.35 to 6.44). Started lesson 7 - completed 7.3</t>
+  </si>
+  <si>
+    <t>D28</t>
   </si>
 </sst>
 </file>
@@ -615,8 +639,8 @@
   </sheetPr>
   <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -815,24 +839,48 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="8">
+        <v>43859</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="8">
+        <v>43860</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="21" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="8">
+        <v>43861</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="8">
+        <v>43862</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="6"/>

</xml_diff>

<commit_message>
D29 update: Completed lesson 7
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70475CC-FF42-C746-9B94-71D46318BC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB94A96-AD38-F241-9DB8-3E3EBD4FE1CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>D28</t>
+  </si>
+  <si>
+    <t>D29</t>
+  </si>
+  <si>
+    <t>Completed lesson 7. Worked on Intel Image classification.</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
   <dimension ref="B1:E51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -883,9 +889,15 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="8">
+        <v>43863</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="6"/>

</xml_diff>

<commit_message>
D30 and 31 updates
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB94A96-AD38-F241-9DB8-3E3EBD4FE1CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33923A60-A8D1-6D4D-BF77-700C60CE81DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>Completed lesson 7. Worked on Intel Image classification.</t>
+  </si>
+  <si>
+    <t>D30</t>
+  </si>
+  <si>
+    <t>Started with lesson 8 - reached 8.3</t>
+  </si>
+  <si>
+    <t>D31</t>
   </si>
 </sst>
 </file>
@@ -272,7 +281,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -299,6 +308,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -645,8 +657,8 @@
   </sheetPr>
   <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -661,11 +673,11 @@
   <sheetData>
     <row r="1" spans="2:5" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="2" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.15">
@@ -900,14 +912,26 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="10">
+        <v>43864</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="25" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+      <c r="B25" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="10">
+        <v>43865</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>

</xml_diff>

<commit_message>
Lesson 8 RNN exercises
</commit_message>
<xml_diff>
--- a/60_days_udacity.xlsx
+++ b/60_days_udacity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thankaselv.kumaresan/Documents/MyFolder/Notes/neural-networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33923A60-A8D1-6D4D-BF77-700C60CE81DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13673E5C-C3A4-7B4F-A7CB-F9FF908A7327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,30 @@
   </si>
   <si>
     <t>D31</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>Watched some videos about RNN</t>
+  </si>
+  <si>
+    <t>D33</t>
+  </si>
+  <si>
+    <t>D34</t>
+  </si>
+  <si>
+    <t>Completed lessons 8.4 and 8.5</t>
+  </si>
+  <si>
+    <t>Completed lessons 8.6 to 8.8</t>
+  </si>
+  <si>
+    <t>D35</t>
+  </si>
+  <si>
+    <t>Completed lesson 8. Participated in study jam from 10.30 AM to midnight. Submitted solutions for binary classification and style transfer problems. Took part in style transfer quizzes. Also, participated in fun activities.</t>
   </si>
 </sst>
 </file>
@@ -658,7 +682,7 @@
   <dimension ref="B1:E51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -934,24 +958,48 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="10">
+        <v>43866</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="27" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="B27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="10">
+        <v>43867</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="28" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="10">
+        <v>43868</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="29" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="B29" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="10">
+        <v>43869</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="30" spans="2:4" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="6"/>

</xml_diff>